<commit_message>
folder structure changed (components) project list and details added
</commit_message>
<xml_diff>
--- a/docs/photo-orders specifications.xlsx
+++ b/docs/photo-orders specifications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\DEV\PhotoStudio\photo-orders\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9419ED56-5958-4A9C-8436-A3E0F86B9827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFB7A63-535E-4C84-81D3-FFA065A22222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="470" windowWidth="27310" windowHeight="19980" activeTab="1" xr2:uid="{96BBC281-1072-44E2-9F10-7FA9F8B9A283}"/>
+    <workbookView xWindow="156" yWindow="108" windowWidth="17856" windowHeight="13308" activeTab="1" xr2:uid="{96BBC281-1072-44E2-9F10-7FA9F8B9A283}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
-  <si>
-    <t>title</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>description</t>
   </si>
@@ -51,18 +48,9 @@
     <t>location</t>
   </si>
   <si>
-    <t>ResolutionAndType</t>
-  </si>
-  <si>
-    <t>Deadline</t>
-  </si>
-  <si>
     <t>numberOfPhotos</t>
   </si>
   <si>
-    <t>EditedOptimized</t>
-  </si>
-  <si>
     <t>Goal</t>
   </si>
   <si>
@@ -114,9 +102,6 @@
     <t>Add / Edit / Delete project</t>
   </si>
   <si>
-    <t>10. Dez. 2024</t>
-  </si>
-  <si>
     <t>1. Dez. 2024</t>
   </si>
   <si>
@@ -126,37 +111,91 @@
     <t>Projekt Details</t>
   </si>
   <si>
-    <t>Networking Workshop</t>
+    <t>travelHours</t>
+  </si>
+  <si>
+    <t>photoShootingHours</t>
+  </si>
+  <si>
+    <t>preparationHours</t>
+  </si>
+  <si>
+    <t>postProductionHours</t>
   </si>
   <si>
     <t>Deliverables</t>
   </si>
   <si>
-    <t>Estimated effort</t>
-  </si>
-  <si>
-    <t>quoteTotal</t>
-  </si>
-  <si>
-    <t>quoteTravelHours</t>
-  </si>
-  <si>
-    <t>quotePreparationHours</t>
-  </si>
-  <si>
-    <t>quotePhotoShootingHours</t>
-  </si>
-  <si>
-    <t>quotePostProductionHours</t>
-  </si>
-  <si>
-    <t>quoteHourlyRateChf</t>
-  </si>
-  <si>
     <t>Baloise Campus, Basel</t>
   </si>
   <si>
-    <t>quoteHoursTotal</t>
+    <t>Networking Workshop Baloise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Networking Workshop auf Dachterasse des Baloise Campus in Basel. Die Photos sollen häuptsächlich den Event und Interaktion der Teilnehmenden untereinander aus einer unabhängigen Beobachterperspektive auffangen, aber auch gelegentliche Gruppenphotos oder Portaits beinhalten. </t>
+  </si>
+  <si>
+    <t>equipment</t>
+  </si>
+  <si>
+    <t>Handfotografie, hauptsächlich mit vorhandenem Licht. Eventuell mit Blitz bei Bedarf.</t>
+  </si>
+  <si>
+    <t>Einfach (Helligkeit, Kontrast, Farbe)</t>
+  </si>
+  <si>
+    <t>selectionByCustomer</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>resolutionAndType</t>
+  </si>
+  <si>
+    <t>editingOptions</t>
+  </si>
+  <si>
+    <t>deadline</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Entwurf | Offerte erstellt | Auftrag erhalten | Foto Auswahl | Rechnung gestellt | Bezahlt</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>Dropdown with existing users</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>project id - generated by firebase</t>
+  </si>
+  <si>
+    <t>Billing</t>
+  </si>
+  <si>
+    <t>Quote</t>
+  </si>
+  <si>
+    <t>totalHours</t>
+  </si>
+  <si>
+    <t>hourlyRateCHF</t>
+  </si>
+  <si>
+    <t>totalCHF</t>
+  </si>
+  <si>
+    <t>issueDate</t>
   </si>
 </sst>
 </file>
@@ -211,7 +250,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -234,11 +273,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -268,6 +322,15 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -619,82 +682,82 @@
   <sheetData>
     <row r="5" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="9" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -704,10 +767,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFA132B-73DE-4806-9DA1-B75E9A05DB9C}">
-  <dimension ref="B4:H36"/>
+  <dimension ref="B4:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -715,7 +778,7 @@
     <col min="1" max="1" width="11.453125" style="1" customWidth="1"/>
     <col min="2" max="2" width="48.6328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="5.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="35.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="70.36328125" style="1" customWidth="1"/>
     <col min="5" max="6" width="8.7265625" style="1"/>
     <col min="7" max="7" width="37.81640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="38.453125" style="1" customWidth="1"/>
@@ -724,159 +787,235 @@
   <sheetData>
     <row r="4" spans="2:8" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="2" t="s">
-        <v>0</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="2:8" ht="57.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
+        <v>43</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G8" s="3"/>
+    </row>
     <row r="9" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="2" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H10" s="4"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="2:8" ht="88.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="10"/>
+    </row>
+    <row r="19" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="26" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="2:8" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D22" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="24" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="26" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" ht="26" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="10"/>
-    </row>
-    <row r="13" spans="2:8" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="18" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="26" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="10"/>
-    </row>
-    <row r="22" spans="2:4" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="2" t="s">
+      <c r="D26" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="28" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="27" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="1">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="29" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="31" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    </row>
+    <row r="29" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="30" spans="2:8" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="12">
+        <v>45636</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="26" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="10"/>
+    </row>
+    <row r="32" spans="2:8" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="33" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D33" s="1">
-        <v>120</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="35" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D35" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="37" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B37" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="39" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="41" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="43" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="45" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B45" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="1">
         <v>720</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="26" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="47" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="12">
+        <v>45616</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="49" spans="2:2" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B49" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" ht="26" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="52" spans="2:2" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>